<commit_message>
fixing 0% bug in work ratio
</commit_message>
<xml_diff>
--- a/config/budget-naming.xlsx
+++ b/config/budget-naming.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\utils\src\excel\evogene-jira-analist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\utils\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5545DF99-436C-4D5A-938E-4E5A2E7342EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DAFB06-C499-42D7-89F2-302D184FF5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
   <si>
     <t>budget</t>
   </si>
@@ -66,18 +66,12 @@
     <t>P82</t>
   </si>
   <si>
-    <t>P999 - General</t>
-  </si>
-  <si>
     <t>AgSeed</t>
   </si>
   <si>
     <t>P300</t>
   </si>
   <si>
-    <t>P999 - General2</t>
-  </si>
-  <si>
     <t>Biomica</t>
   </si>
   <si>
@@ -187,6 +181,27 @@
   </si>
   <si>
     <t>Crispril</t>
+  </si>
+  <si>
+    <t>P999 - Agseed</t>
+  </si>
+  <si>
+    <t>P999 - Laviebio</t>
+  </si>
+  <si>
+    <t>P999 - Biomica</t>
+  </si>
+  <si>
+    <t>P290</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>P000</t>
+  </si>
+  <si>
+    <t>Out of Office</t>
   </si>
 </sst>
 </file>
@@ -506,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A36" zoomScale="142" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -547,7 +562,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -571,7 +586,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -579,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -627,231 +642,255 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
         <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing bugs and updated data for current year
</commit_message>
<xml_diff>
--- a/config/budget-naming.xlsx
+++ b/config/budget-naming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\utils\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DAFB06-C499-42D7-89F2-302D184FF5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD40C42-DB3B-4BFF-9D8C-84C1C0AD9644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14175" yWindow="2055" windowWidth="14280" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
   <si>
     <t>budget</t>
   </si>
@@ -202,16 +202,64 @@
   </si>
   <si>
     <t>Out of Office</t>
+  </si>
+  <si>
+    <t>P33</t>
+  </si>
+  <si>
+    <t>P85</t>
+  </si>
+  <si>
+    <t>P86</t>
+  </si>
+  <si>
+    <t>P258</t>
+  </si>
+  <si>
+    <t>Casterra</t>
+  </si>
+  <si>
+    <t>P402</t>
+  </si>
+  <si>
+    <t>P403</t>
+  </si>
+  <si>
+    <t>P404</t>
+  </si>
+  <si>
+    <t>Generator</t>
+  </si>
+  <si>
+    <t>P272</t>
+  </si>
+  <si>
+    <t>The Kitchen</t>
+  </si>
+  <si>
+    <t>P401</t>
+  </si>
+  <si>
+    <t>Corp4clima</t>
+  </si>
+  <si>
+    <t>P400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A36" zoomScale="142" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" zoomScale="142" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -578,15 +626,15 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -594,7 +642,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -602,7 +650,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -610,7 +658,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -618,7 +666,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -626,7 +674,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -634,7 +682,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -642,47 +690,47 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -690,7 +738,7 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -698,39 +746,39 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -738,7 +786,7 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -746,7 +794,7 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -754,7 +802,7 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -762,103 +810,103 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>51</v>
+      <c r="A35" t="s">
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>43</v>
+      <c r="A38" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>43</v>
+      <c r="A39" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -866,34 +914,115 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>58</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B49" t="s">
         <v>57</v>
       </c>
     </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding p21, p23 to configuration, fixng latest sprint bugs
</commit_message>
<xml_diff>
--- a/config/budget-naming.xlsx
+++ b/config/budget-naming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\utils\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E55284-C96E-4F6F-B22C-7CFB12201371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FE7DFB-63D9-45E1-B308-A6CA470C590A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
   <si>
     <t>budget</t>
   </si>
@@ -169,6 +169,24 @@
   </si>
   <si>
     <t>94. VERB (165)</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>P403</t>
+  </si>
+  <si>
+    <t>96. Canonic (213, 216)</t>
+  </si>
+  <si>
+    <t>P216</t>
+  </si>
+  <si>
+    <t>P213</t>
+  </si>
+  <si>
+    <t>P21</t>
   </si>
 </sst>
 </file>
@@ -524,15 +542,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A25" zoomScale="142" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A33" zoomScale="142" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -549,7 +567,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -557,7 +575,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -565,7 +583,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -573,7 +591,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -581,23 +599,23 @@
         <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -605,7 +623,7 @@
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -613,7 +631,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -621,7 +639,7 @@
         <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -629,23 +647,23 @@
         <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -653,7 +671,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -661,135 +679,175 @@
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>41</v>
+      <c r="A25" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>42</v>
+      <c r="A27" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding BVA report by eork cost
</commit_message>
<xml_diff>
--- a/config/budget-naming.xlsx
+++ b/config/budget-naming.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\utils\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FE7DFB-63D9-45E1-B308-A6CA470C590A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7199D6FD-ABBB-42D1-A870-786A28CB5D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18930" yWindow="3210" windowWidth="14370" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>budget</t>
   </si>
@@ -138,9 +147,6 @@
     <t>9. MicroBoost (265, 273)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1. CPB 279 PROJECTS</t>
-  </si>
-  <si>
     <t>2. CPB-271 UPKEEP</t>
   </si>
   <si>
@@ -187,6 +193,18 @@
   </si>
   <si>
     <t>P21</t>
+  </si>
+  <si>
+    <t>P282</t>
+  </si>
+  <si>
+    <t>1. CPB 279 PROJECTS</t>
+  </si>
+  <si>
+    <t>P999 â€“ General (Biomica)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P997-271 - Upkeep Computational </t>
   </si>
 </sst>
 </file>
@@ -216,7 +234,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -254,14 +272,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A33" zoomScale="142" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A39" zoomScale="142" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -567,7 +621,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -583,7 +637,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -660,18 +714,18 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -679,7 +733,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -687,7 +741,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -695,15 +749,15 @@
         <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,15 +765,15 @@
         <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -727,127 +781,151 @@
         <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>52</v>
+    </row>
+    <row r="39" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>